<commit_message>
changes in htmls and views.py
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Computer Achitecture and Organisation</t>
   </si>
@@ -73,31 +73,7 @@
     <t>Applications developer</t>
   </si>
   <si>
-    <t>1,2</t>
-  </si>
-  <si>
-    <t>1,9</t>
-  </si>
-  <si>
-    <t>1,3</t>
-  </si>
-  <si>
-    <t>1,1</t>
-  </si>
-  <si>
-    <t>1,5</t>
-  </si>
-  <si>
-    <t>1,4</t>
-  </si>
-  <si>
     <t>Data analyst</t>
-  </si>
-  <si>
-    <t>1,7</t>
-  </si>
-  <si>
-    <t>1,6</t>
   </si>
   <si>
     <t>Database administrator</t>
@@ -146,13 +122,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -168,12 +143,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -197,7 +169,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="36.71"/>
+    <col customWidth="1" min="1" max="1" width="25.71"/>
     <col customWidth="1" min="2" max="2" width="33.71"/>
     <col customWidth="1" min="3" max="3" width="13.71"/>
     <col customWidth="1" min="4" max="4" width="17.71"/>
@@ -286,11 +258,11 @@
       <c r="B2">
         <v>0.0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
+      <c r="C2">
+        <v>1.0</v>
+      </c>
+      <c r="D2">
+        <v>1.0</v>
       </c>
       <c r="E2">
         <v>0.0</v>
@@ -298,11 +270,11 @@
       <c r="F2">
         <v>0.0</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>23</v>
+      <c r="G2">
+        <v>1.0</v>
+      </c>
+      <c r="H2">
+        <v>1.0</v>
       </c>
       <c r="I2">
         <v>0.0</v>
@@ -319,8 +291,8 @@
       <c r="M2">
         <v>0.0</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>24</v>
+      <c r="N2">
+        <v>1.0</v>
       </c>
       <c r="O2">
         <v>0.0</v>
@@ -331,8 +303,8 @@
       <c r="Q2">
         <v>0.0</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>25</v>
+      <c r="R2">
+        <v>1.0</v>
       </c>
       <c r="S2">
         <v>0.0</v>
@@ -343,22 +315,22 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>0.0</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>25</v>
+      <c r="C3">
+        <v>1.0</v>
       </c>
       <c r="D3">
         <v>0.0</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
+      <c r="E3">
+        <v>1.0</v>
+      </c>
+      <c r="F3">
+        <v>1.0</v>
       </c>
       <c r="G3">
         <v>0.0</v>
@@ -375,14 +347,14 @@
       <c r="K3">
         <v>0.0</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>20</v>
+      <c r="L3">
+        <v>1.0</v>
       </c>
       <c r="M3">
         <v>0.0</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>22</v>
+      <c r="N3">
+        <v>1.0</v>
       </c>
       <c r="O3">
         <v>0.0</v>
@@ -393,11 +365,11 @@
       <c r="Q3">
         <v>0.0</v>
       </c>
-      <c r="R3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>24</v>
+      <c r="R3">
+        <v>1.0</v>
+      </c>
+      <c r="S3">
+        <v>1.0</v>
       </c>
       <c r="T3">
         <v>0.0</v>
@@ -405,13 +377,13 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>1.0</v>
+      </c>
+      <c r="C4">
+        <v>1.0</v>
       </c>
       <c r="D4">
         <v>0.0</v>
@@ -419,14 +391,14 @@
       <c r="E4">
         <v>0.0</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>20</v>
+      <c r="F4">
+        <v>1.0</v>
+      </c>
+      <c r="G4">
+        <v>1.0</v>
+      </c>
+      <c r="H4">
+        <v>1.0</v>
       </c>
       <c r="I4">
         <v>0.0</v>
@@ -455,8 +427,8 @@
       <c r="Q4">
         <v>0.0</v>
       </c>
-      <c r="R4" s="1" t="s">
-        <v>23</v>
+      <c r="R4">
+        <v>1.0</v>
       </c>
       <c r="S4">
         <v>0.0</v>
@@ -467,16 +439,16 @@
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>0.0</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>24</v>
+      <c r="C5">
+        <v>1.0</v>
+      </c>
+      <c r="D5">
+        <v>1.0</v>
       </c>
       <c r="E5">
         <v>0.0</v>
@@ -484,11 +456,11 @@
       <c r="F5">
         <v>0.0</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>22</v>
+      <c r="G5">
+        <v>1.0</v>
+      </c>
+      <c r="H5">
+        <v>1.0</v>
       </c>
       <c r="I5">
         <v>0.0</v>
@@ -496,20 +468,20 @@
       <c r="J5">
         <v>0.0</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>20</v>
+      <c r="K5">
+        <v>1.0</v>
       </c>
       <c r="L5">
         <v>0.0</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>21</v>
+      <c r="M5">
+        <v>1.0</v>
+      </c>
+      <c r="N5">
+        <v>1.0</v>
+      </c>
+      <c r="O5">
+        <v>1.0</v>
       </c>
       <c r="P5">
         <v>0.0</v>
@@ -517,11 +489,11 @@
       <c r="Q5">
         <v>1.0</v>
       </c>
-      <c r="R5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>23</v>
+      <c r="R5">
+        <v>1.0</v>
+      </c>
+      <c r="S5">
+        <v>0.0</v>
       </c>
       <c r="T5">
         <v>0.0</v>
@@ -529,7 +501,7 @@
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>0.0</v>
@@ -591,7 +563,7 @@
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>0.0</v>
@@ -653,7 +625,7 @@
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>0.0</v>
@@ -715,7 +687,7 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>0.0</v>
@@ -777,7 +749,7 @@
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>1.0</v>
@@ -839,7 +811,7 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>1.0</v>
@@ -901,7 +873,7 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>0.0</v>
@@ -963,7 +935,7 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>0.0</v>
@@ -1025,7 +997,7 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>0.0</v>
@@ -1087,7 +1059,7 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>0.0</v>
@@ -1149,7 +1121,7 @@
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>1.0</v>
@@ -1211,7 +1183,7 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>1.0</v>

</xml_diff>